<commit_message>
Deploying to gh-pages from  @ 41e7ae1fae1d11b382ad2e1f1bd8a014d0c5cf58 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-2-1.xlsx
+++ b/assets/excel/2021_1-2-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DDDA96-51FD-402A-B146-EDDCCEBEDE59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4E9C1F-E2DE-468D-916F-ABC9D19BE7EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{E8B70F38-DE1B-4179-B181-7CCB39045086}"/>
   </bookViews>
@@ -231,7 +231,7 @@
     <numFmt numFmtId="164" formatCode="###\ ###\ ##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,6 +302,16 @@
       <sz val="6"/>
       <color theme="10"/>
       <name val="NDSFrutiger 45 Light"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color indexed="8"/>
+      <name val="NDSFrutiger 55 Roman"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="NDSFrutiger 55 Roman"/>
     </font>
   </fonts>
   <fills count="2">
@@ -431,7 +441,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -485,18 +495,6 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -527,6 +525,14 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -545,14 +551,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Link" xfId="4" builtinId="8"/>
@@ -874,8 +885,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:R70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +897,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="P1"/>
@@ -894,20 +905,20 @@
     </row>
     <row r="2" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="32" t="s">
         <v>1</v>
       </c>
       <c r="P3"/>
       <c r="Q3"/>
     </row>
     <row r="4" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="31" t="s">
         <v>2</v>
       </c>
       <c r="P4"/>
       <c r="Q4"/>
     </row>
-    <row r="6" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="35" t="s">
         <v>3</v>
       </c>
@@ -930,7 +941,7 @@
       <c r="Q6" s="38"/>
       <c r="R6" s="39"/>
     </row>
-    <row r="7" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="36"/>
       <c r="C7" s="2">
         <v>2005</v>
@@ -1002,7 +1013,7 @@
       <c r="Q8" s="40"/>
       <c r="R8" s="40"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>1</v>
       </c>
@@ -1055,7 +1066,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>61</v>
       </c>
@@ -1108,7 +1119,7 @@
         <v>30950</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>62</v>
       </c>
@@ -1161,7 +1172,7 @@
         <v>20785</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>63</v>
       </c>
@@ -1214,7 +1225,7 @@
         <v>20265</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>6</v>
       </c>
@@ -1267,7 +1278,7 @@
         <v>12955</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>7</v>
       </c>
@@ -1320,7 +1331,7 @@
         <v>13830</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>8</v>
       </c>
@@ -1373,7 +1384,7 @@
         <v>6760</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>9</v>
       </c>
@@ -1426,7 +1437,7 @@
         <v>9310</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>10</v>
       </c>
@@ -1479,7 +1490,7 @@
         <v>11985</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>11</v>
       </c>
@@ -1532,7 +1543,7 @@
         <v>7860</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>12</v>
       </c>
@@ -1585,60 +1596,60 @@
         <v>32265</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="41">
         <v>99536</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="41">
         <v>97675</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="41">
         <v>95376</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="41">
         <v>93595</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="41">
         <v>93485</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="41">
         <v>93067</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="41">
         <v>94569</v>
       </c>
-      <c r="J20" s="19">
+      <c r="J20" s="41">
         <v>97812</v>
       </c>
-      <c r="K20" s="19">
+      <c r="K20" s="41">
         <v>104548</v>
       </c>
-      <c r="L20" s="19">
+      <c r="L20" s="41">
         <v>112534</v>
       </c>
-      <c r="M20" s="19">
+      <c r="M20" s="41">
         <v>130933</v>
       </c>
-      <c r="N20" s="20">
+      <c r="N20" s="42">
         <v>145155</v>
       </c>
-      <c r="O20" s="21">
+      <c r="O20" s="43">
         <v>151170</v>
       </c>
-      <c r="P20" s="22">
+      <c r="P20" s="44">
         <v>158180</v>
       </c>
-      <c r="Q20" s="22">
+      <c r="Q20" s="44">
         <v>165000</v>
       </c>
-      <c r="R20" s="22">
+      <c r="R20" s="44">
         <v>166960</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>13</v>
       </c>
@@ -1691,7 +1702,7 @@
         <v>185675</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>14</v>
       </c>
@@ -1744,7 +1755,7 @@
         <v>112125</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>15</v>
       </c>
@@ -1797,7 +1808,7 @@
         <v>73550</v>
       </c>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
         <v>16</v>
       </c>
@@ -1850,7 +1861,7 @@
         <v>19395</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>17</v>
       </c>
@@ -1903,7 +1914,7 @@
         <v>17460</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>18</v>
       </c>
@@ -1956,7 +1967,7 @@
         <v>25525</v>
       </c>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>19</v>
       </c>
@@ -2009,7 +2020,7 @@
         <v>4490</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>20</v>
       </c>
@@ -2062,7 +2073,7 @@
         <v>10560</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>21</v>
       </c>
@@ -2115,60 +2126,60 @@
         <v>14755</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="41">
         <v>167595</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="41">
         <v>165870</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E30" s="41">
         <v>164632</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F30" s="41">
         <v>161409</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="41">
         <v>160303</v>
       </c>
-      <c r="H30" s="19">
+      <c r="H30" s="41">
         <v>160800</v>
       </c>
-      <c r="I30" s="19">
+      <c r="I30" s="41">
         <v>164319</v>
       </c>
-      <c r="J30" s="19">
+      <c r="J30" s="41">
         <v>170246</v>
       </c>
-      <c r="K30" s="19">
+      <c r="K30" s="41">
         <v>181572</v>
       </c>
-      <c r="L30" s="19">
+      <c r="L30" s="41">
         <v>195197</v>
       </c>
-      <c r="M30" s="19">
+      <c r="M30" s="41">
         <v>223573</v>
       </c>
-      <c r="N30" s="20">
+      <c r="N30" s="42">
         <v>247535</v>
       </c>
-      <c r="O30" s="21">
+      <c r="O30" s="43">
         <v>257705</v>
       </c>
-      <c r="P30" s="22">
+      <c r="P30" s="44">
         <v>268505</v>
       </c>
-      <c r="Q30" s="22">
+      <c r="Q30" s="44">
         <v>274635</v>
       </c>
-      <c r="R30" s="22">
+      <c r="R30" s="44">
         <v>277860</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>22</v>
       </c>
@@ -2221,7 +2232,7 @@
         <v>14300</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
         <v>23</v>
       </c>
@@ -2274,7 +2285,7 @@
         <v>13410</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
         <v>24</v>
       </c>
@@ -2327,7 +2338,7 @@
         <v>22685</v>
       </c>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
         <v>25</v>
       </c>
@@ -2380,7 +2391,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
         <v>26</v>
       </c>
@@ -2433,7 +2444,7 @@
         <v>13095</v>
       </c>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
         <v>27</v>
       </c>
@@ -2486,7 +2497,7 @@
         <v>6980</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
         <v>28</v>
       </c>
@@ -2539,7 +2550,7 @@
         <v>12055</v>
       </c>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
         <v>29</v>
       </c>
@@ -2592,7 +2603,7 @@
         <v>12750</v>
       </c>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
         <v>30</v>
       </c>
@@ -2645,7 +2656,7 @@
         <v>19980</v>
       </c>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
         <v>31</v>
       </c>
@@ -2698,7 +2709,7 @@
         <v>6015</v>
       </c>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="s">
         <v>32</v>
       </c>
@@ -2751,60 +2762,60 @@
         <v>11465</v>
       </c>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:18" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="19">
+      <c r="C42" s="41">
         <v>69762</v>
       </c>
-      <c r="D42" s="19">
+      <c r="D42" s="41">
         <v>68586</v>
       </c>
-      <c r="E42" s="19">
+      <c r="E42" s="41">
         <v>67702</v>
       </c>
-      <c r="F42" s="19">
+      <c r="F42" s="41">
         <v>67279</v>
       </c>
-      <c r="G42" s="19">
+      <c r="G42" s="41">
         <v>67529</v>
       </c>
-      <c r="H42" s="19">
+      <c r="H42" s="41">
         <v>67951</v>
       </c>
-      <c r="I42" s="19">
+      <c r="I42" s="41">
         <v>69224</v>
       </c>
-      <c r="J42" s="19">
+      <c r="J42" s="41">
         <v>71972</v>
       </c>
-      <c r="K42" s="19">
+      <c r="K42" s="41">
         <v>77840</v>
       </c>
-      <c r="L42" s="19">
+      <c r="L42" s="41">
         <v>85566</v>
       </c>
-      <c r="M42" s="19">
+      <c r="M42" s="41">
         <v>101355</v>
       </c>
-      <c r="N42" s="20">
+      <c r="N42" s="42">
         <v>116020</v>
       </c>
-      <c r="O42" s="21">
+      <c r="O42" s="43">
         <v>120060</v>
       </c>
-      <c r="P42" s="22">
+      <c r="P42" s="44">
         <v>126195</v>
       </c>
-      <c r="Q42" s="22">
+      <c r="Q42" s="44">
         <v>132025</v>
       </c>
-      <c r="R42" s="22">
+      <c r="R42" s="44">
         <v>135635</v>
       </c>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="s">
         <v>33</v>
       </c>
@@ -2857,7 +2868,7 @@
         <v>13710</v>
       </c>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
         <v>34</v>
       </c>
@@ -2910,7 +2921,7 @@
         <v>6040</v>
       </c>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
         <v>35</v>
       </c>
@@ -2963,7 +2974,7 @@
         <v>19145</v>
       </c>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="s">
         <v>36</v>
       </c>
@@ -3016,7 +3027,7 @@
         <v>25420</v>
       </c>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
         <v>37</v>
       </c>
@@ -3069,7 +3080,7 @@
         <v>8800</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
@@ -3122,7 +3133,7 @@
         <v>8735</v>
       </c>
     </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="10" t="s">
         <v>39</v>
       </c>
@@ -3175,7 +3186,7 @@
         <v>11465</v>
       </c>
     </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
         <v>40</v>
       </c>
@@ -3228,7 +3239,7 @@
         <v>20565</v>
       </c>
     </row>
-    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
         <v>41</v>
       </c>
@@ -3281,7 +3292,7 @@
         <v>41090</v>
       </c>
     </row>
-    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="s">
         <v>42</v>
       </c>
@@ -3334,7 +3345,7 @@
         <v>4905</v>
       </c>
     </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="10" t="s">
         <v>43</v>
       </c>
@@ -3387,7 +3398,7 @@
         <v>22410</v>
       </c>
     </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
         <v>44</v>
       </c>
@@ -3440,7 +3451,7 @@
         <v>15200</v>
       </c>
     </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="10" t="s">
         <v>45</v>
       </c>
@@ -3493,7 +3504,7 @@
         <v>12850</v>
       </c>
     </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
         <v>46</v>
       </c>
@@ -3546,7 +3557,7 @@
         <v>34995</v>
       </c>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>47</v>
       </c>
@@ -3599,7 +3610,7 @@
         <v>21370</v>
       </c>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>48</v>
       </c>
@@ -3652,7 +3663,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>49</v>
       </c>
@@ -3705,151 +3716,151 @@
         <v>2915</v>
       </c>
     </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:18" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B60" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C60" s="19">
+      <c r="C60" s="41">
         <v>124593</v>
       </c>
-      <c r="D60" s="19">
+      <c r="D60" s="41">
         <v>126626</v>
       </c>
-      <c r="E60" s="19">
+      <c r="E60" s="41">
         <v>129389</v>
       </c>
-      <c r="F60" s="19">
+      <c r="F60" s="41">
         <v>130858</v>
       </c>
-      <c r="G60" s="19">
+      <c r="G60" s="41">
         <v>132319</v>
       </c>
-      <c r="H60" s="19">
+      <c r="H60" s="41">
         <v>136335</v>
       </c>
-      <c r="I60" s="19">
+      <c r="I60" s="41">
         <v>142571</v>
       </c>
-      <c r="J60" s="19">
+      <c r="J60" s="41">
         <v>152042</v>
       </c>
-      <c r="K60" s="19">
+      <c r="K60" s="41">
         <v>161729</v>
       </c>
-      <c r="L60" s="19">
+      <c r="L60" s="41">
         <v>177691</v>
       </c>
-      <c r="M60" s="19">
+      <c r="M60" s="41">
         <v>207956</v>
       </c>
-      <c r="N60" s="20">
+      <c r="N60" s="42">
         <v>236470</v>
       </c>
-      <c r="O60" s="21">
+      <c r="O60" s="43">
         <v>247925</v>
       </c>
-      <c r="P60" s="22">
+      <c r="P60" s="44">
         <v>260205</v>
       </c>
-      <c r="Q60" s="22">
+      <c r="Q60" s="44">
         <v>269505</v>
       </c>
-      <c r="R60" s="22">
+      <c r="R60" s="44">
         <v>277435</v>
       </c>
     </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:18" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B61" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C61" s="19">
+      <c r="C61" s="41">
         <v>461486</v>
       </c>
-      <c r="D61" s="19">
+      <c r="D61" s="41">
         <v>458757</v>
       </c>
-      <c r="E61" s="19">
+      <c r="E61" s="41">
         <v>457099</v>
       </c>
-      <c r="F61" s="19">
+      <c r="F61" s="41">
         <v>453141</v>
       </c>
-      <c r="G61" s="19">
+      <c r="G61" s="41">
         <v>453636</v>
       </c>
-      <c r="H61" s="19">
+      <c r="H61" s="41">
         <v>458153</v>
       </c>
-      <c r="I61" s="19">
+      <c r="I61" s="41">
         <v>470683</v>
       </c>
-      <c r="J61" s="19">
+      <c r="J61" s="41">
         <v>492072</v>
       </c>
-      <c r="K61" s="19">
+      <c r="K61" s="41">
         <v>525689</v>
       </c>
-      <c r="L61" s="19">
+      <c r="L61" s="41">
         <v>570988</v>
       </c>
-      <c r="M61" s="19">
+      <c r="M61" s="41">
         <v>663817</v>
       </c>
-      <c r="N61" s="20">
+      <c r="N61" s="42">
         <v>745185</v>
       </c>
-      <c r="O61" s="21">
+      <c r="O61" s="43">
         <v>776860</v>
       </c>
-      <c r="P61" s="22">
+      <c r="P61" s="44">
         <v>813080</v>
       </c>
-      <c r="Q61" s="22">
+      <c r="Q61" s="44">
         <v>841165</v>
       </c>
-      <c r="R61" s="22">
+      <c r="R61" s="44">
         <v>857895</v>
       </c>
     </row>
-    <row r="62" spans="2:18" s="26" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:18" s="22" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="12"/>
-      <c r="D62" s="23"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="23"/>
-      <c r="H62" s="23"/>
-      <c r="I62" s="23"/>
-      <c r="J62" s="23"/>
-      <c r="K62" s="23"/>
-      <c r="L62" s="23"/>
-      <c r="M62" s="23"/>
-      <c r="N62" s="23"/>
-      <c r="O62" s="24"/>
-      <c r="P62" s="24"/>
-      <c r="Q62" s="25"/>
-      <c r="R62" s="25"/>
-    </row>
-    <row r="63" spans="2:18" s="29" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="27" t="s">
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="19"/>
+      <c r="K62" s="19"/>
+      <c r="L62" s="19"/>
+      <c r="M62" s="19"/>
+      <c r="N62" s="19"/>
+      <c r="O62" s="20"/>
+      <c r="P62" s="20"/>
+      <c r="Q62" s="21"/>
+      <c r="R62" s="21"/>
+    </row>
+    <row r="63" spans="2:18" s="25" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="27"/>
-      <c r="H63" s="27"/>
-      <c r="I63" s="27"/>
-      <c r="J63" s="27"/>
-      <c r="K63" s="27"/>
-      <c r="L63" s="27"/>
-      <c r="N63" s="27"/>
-      <c r="O63" s="23"/>
-      <c r="P63" s="23"/>
-      <c r="Q63" s="28"/>
-      <c r="R63" s="28"/>
-    </row>
-    <row r="64" spans="2:18" s="29" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="23"/>
+      <c r="G63" s="23"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="23"/>
+      <c r="J63" s="23"/>
+      <c r="K63" s="23"/>
+      <c r="L63" s="23"/>
+      <c r="N63" s="23"/>
+      <c r="O63" s="19"/>
+      <c r="P63" s="19"/>
+      <c r="Q63" s="24"/>
+      <c r="R63" s="24"/>
+    </row>
+    <row r="64" spans="2:18" s="25" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
@@ -3861,49 +3872,50 @@
       <c r="K64" s="13"/>
       <c r="L64" s="13"/>
       <c r="M64" s="13"/>
-      <c r="N64" s="27"/>
-      <c r="O64" s="30"/>
-      <c r="P64" s="30"/>
-      <c r="Q64" s="31"/>
-      <c r="R64" s="31"/>
+      <c r="N64" s="23"/>
+      <c r="O64" s="26"/>
+      <c r="P64" s="26"/>
+      <c r="Q64" s="27"/>
+      <c r="R64" s="27"/>
     </row>
     <row r="65" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="32"/>
-      <c r="H65" s="32"/>
-      <c r="I65" s="32"/>
-      <c r="J65" s="32"/>
-      <c r="K65" s="32"/>
-      <c r="L65" s="32"/>
-      <c r="M65" s="32"/>
-      <c r="N65" s="27"/>
-      <c r="O65" s="33"/>
-      <c r="P65" s="33"/>
-      <c r="Q65" s="34"/>
-      <c r="R65" s="34"/>
-    </row>
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="28"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="28"/>
+      <c r="I65" s="28"/>
+      <c r="J65" s="28"/>
+      <c r="K65" s="28"/>
+      <c r="L65" s="28"/>
+      <c r="M65" s="28"/>
+      <c r="N65" s="23"/>
+      <c r="O65" s="29"/>
+      <c r="P65" s="29"/>
+      <c r="Q65" s="30"/>
+      <c r="R65" s="30"/>
+    </row>
+    <row r="66" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="43" t="s">
+      <c r="B67" s="33" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="68" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="43" t="s">
+      <c r="B68" s="33" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="69" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="43" t="s">
+      <c r="B69" s="33" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="70" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="44" t="s">
+      <c r="B70" s="34" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>